<commit_message>
Created catering vehicles and moved refuel to correct location. Also changed reversing out to be optional
</commit_message>
<xml_diff>
--- a/Base_Mesh_4.xlsx
+++ b/Base_Mesh_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimLe\PycharmProjects\JIP_ApronSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A59DD9D-D025-40DD-B77F-FAE021F43089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADD8585-5AF2-4FF4-B17B-FD35DB7FBCF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,8 +343,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:GJ158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CJ53" sqref="CJ52:CM53"/>
+    <sheetView tabSelected="1" topLeftCell="Z33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BU60" sqref="BU60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>